<commit_message>
19-01-25 Updated views.py (Date search bug fix)
</commit_message>
<xml_diff>
--- a/FlaskServer/static/excel/생산계획.xlsx
+++ b/FlaskServer/static/excel/생산계획.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -66,7 +66,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -145,25 +145,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>